<commit_message>
update code file imports to match names to provided files
</commit_message>
<xml_diff>
--- a/data/tables&plots/redacted_tables.xlsx
+++ b/data/tables&plots/redacted_tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2-Academia\capstone_20729_LSE\data\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2-Academia\capstone_20729_LSE\data\tables&amp;plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF14AC8D-4D3E-4056-8221-8C57EFCAB5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C72D1E-BB32-46B1-B006-1ADD631F7A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{32EC32C4-8D5C-AA4A-A655-0A5FA94F8E87}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{32EC32C4-8D5C-AA4A-A655-0A5FA94F8E87}"/>
   </bookViews>
   <sheets>
     <sheet name="ABOUT" sheetId="9" r:id="rId1"/>
@@ -1634,16 +1634,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>639535</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
+      <xdr:colOff>368753</xdr:colOff>
       <xdr:row>159</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1673,8 +1673,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="685800" y="15020925"/>
-          <a:ext cx="8639175" cy="16897350"/>
+          <a:off x="639535" y="15294429"/>
+          <a:ext cx="8573861" cy="17240250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1838,7 +1838,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1899,7 +1899,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1960,7 +1960,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2026,7 +2026,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2087,7 +2087,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2148,7 +2148,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2209,7 +2209,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2270,7 +2270,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2615,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EE4E72-99C9-4E6A-853C-1BF19A8B89B3}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -13372,7 +13372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7DF77D-6E62-4C77-9467-B0D4951AD54B}">
   <dimension ref="B3:AG124"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Z68" sqref="Z68"/>
     </sheetView>
   </sheetViews>

</xml_diff>